<commit_message>
Update documentation and add gitignore for legacy CSV files
Co-authored-by: trashduty <173416117+trashduty@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/master_game_tracking.xlsx
+++ b/master_game_tracking.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,6 +665,11 @@
           <t>spread_result</t>
         </is>
       </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>game_date</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -797,6 +802,11 @@
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -933,6 +943,11 @@
       <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1069,6 +1084,11 @@
       <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="inlineStr"/>
       <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1205,6 +1225,11 @@
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implement historical CSV data migration with backup and validation
Co-authored-by: trashduty <173416117+trashduty@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/master_game_tracking.xlsx
+++ b/master_game_tracking.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU5"/>
+  <dimension ref="A1:AU15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1226,6 +1226,800 @@
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="inlineStr"/>
       <c r="AU5" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Nov 11 07:00PM ET</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Morehead St Eagles</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>24.65</v>
+      </c>
+      <c r="G6" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0400692258560322</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Nov 11 07:00PM ET</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Army Knights</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="G7" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0481402508762097</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
+      <c r="AT7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Nov 11 07:30PM ET</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Eastern Illinois Panthers</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20.05</v>
+      </c>
+      <c r="G8" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0432973911604778</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Nov 11 08:00PM ET</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Maryland-Eastern Shore Hawks</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>30.55</v>
+      </c>
+      <c r="G9" t="n">
+        <v>34</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0524691789372875</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Nov 11 08:00PM ET</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Wofford Terriers</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>22.45</v>
+      </c>
+      <c r="G10" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0400692258560322</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Nov 11 08:30PM ET</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Illinois Fighting Illini</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-9.15</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-6</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.0558464163570781</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nov 11 09:00PM ET</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Northern Arizona Lumberjacks</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>29.75</v>
+      </c>
+      <c r="G12" t="n">
+        <v>33</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0627477276062155</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr"/>
+      <c r="AS12" t="inlineStr"/>
+      <c r="AT12" t="inlineStr"/>
+      <c r="AU12" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Nov 11 09:00PM ET</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Delaware Blue Hens</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>36</v>
+      </c>
+      <c r="F13" t="n">
+        <v>29.65</v>
+      </c>
+      <c r="G13" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>36</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0558464163570781</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Nov 11 09:00PM ET</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Hampton Pirates</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="G14" t="n">
+        <v>21</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.0604251709358326</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
+      <c r="AU14" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Vanderbilt Commodores vs. Eastern Kentucky Colonels</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Nov 12 08:00PM ET</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Eastern Kentucky Colonels</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>23.75</v>
+      </c>
+      <c r="G15" t="n">
+        <v>27</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5796559401666019</v>
+      </c>
+      <c r="I15" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.0650928333704854</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="L15" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="M15" t="n">
+        <v>25</v>
+      </c>
+      <c r="N15" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="O15" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.0179603331218772</v>
+      </c>
+      <c r="X15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>171</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>166.276065551855</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>169</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>171</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>166</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>167</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>166.55213110371</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>156.94</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>0.4624333836521225</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>0.5225634700046342</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>-0.07673712326031989</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>0.0176129749551292</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="inlineStr"/>
+      <c r="AU15" t="inlineStr">
         <is>
           <t>2025-11-12</t>
         </is>
@@ -1242,7 +2036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1253,207 +2047,666 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Game Time</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Game</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Game Time</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>market_total</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>model_total</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Over Total Edge</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Under Total Edge</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>over_consensus_flag</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>under_consensus_flag</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Team</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>total_category</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>market_spread</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>model_spread</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Predicted Outcome</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Spread Cover Probability</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Opening Spread</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Edge For Covering Spread</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Spread Std. Dev.</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>spread_barttorvik</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>spread_kenpom</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>spread_evanmiya</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>spread_hasla</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Moneyline Win Probability</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Opening Moneyline</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Devigged Probability</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Moneyline Edge</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Moneyline Std. Dev.</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>win_prob_barttorvik</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>win_prob_kenpom</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>win_prob_evanmiya</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>spread_category</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>market_total</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>model_total</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>average_total</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>theoddsapi_total</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Totals Std. Dev.</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>projected_total_barttorvik</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>projected_total_kenpom</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>projected_total_evanmiya</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>projected_total_hasla</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Over Cover Probability</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Under Cover Probability</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Over Total Edge</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Under Total Edge</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>spread_consensus_flag</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>moneyline_consensus_flag</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>over_consensus_flag</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>under_consensus_flag</t>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>actual_score_team1</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>actual_score_team2</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>actual_total</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>over_result</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>under_result</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>game_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Nov 11 07:00PM ET</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Providence Friars vs. Pennsylvania Quakers</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>173.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>163.9206912013885</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.0837691007298096</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0361500531107619</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Nov 11 07:00PM ET</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Florida Gators vs. Florida St Seminoles</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>167.407946090007</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.1059902260430259</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0435904388870667</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nov 11 08:00PM ET</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Louisville Cardinals vs. Kentucky Wildcats</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>173.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>164.0360081674465</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.0857954199913341</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0381763723722864</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Nov 11 10:00PM ET</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sacramento St Hornets vs. UC Santa Barbara Gauchos</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>160.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>148.438073759212</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.1011160379673318</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0534969903482841</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Nov 12 08:00PM ET</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Oklahoma St Cowboys vs. Prairie View Panthers</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>170</v>
+      </c>
+      <c r="D6" t="n">
+        <v>162.05</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.0958981417961835</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0375692556952089</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Prairie View Panthers</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>32</v>
+      </c>
+      <c r="L6" t="n">
+        <v>29.35</v>
+      </c>
+      <c r="M6" t="n">
+        <v>31</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5320425632110974</v>
+      </c>
+      <c r="O6" t="n">
+        <v>32</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.0082330394015736</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="R6" t="n">
+        <v>32</v>
+      </c>
+      <c r="S6" t="n">
+        <v>28</v>
+      </c>
+      <c r="T6" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="U6" t="n">
+        <v>25.9</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.0069001475695512</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>167</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>170</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>164</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>160</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>165.681167456194</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>160.1</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.4474808536376065</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.537569255695209</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial exploration - understanding game grading issue
Co-authored-by: trashduty <173416117+trashduty@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/master_game_tracking.xlsx
+++ b/master_game_tracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Spreads" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Totals" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Spreads" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Totals" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU15"/>
+  <dimension ref="A1:AU17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2024,6 +2024,276 @@
           <t>2025-11-12</t>
         </is>
       </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Virginia Tech Hokies vs. Saint Joseph's Hawks</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Nov 12 07:00PM ET</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Saint Joseph's Hawks</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>13</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="G16" t="n">
+        <v>11</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5638787496655561</v>
+      </c>
+      <c r="I16" t="n">
+        <v>13</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0400692258560322</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="L16" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="M16" t="n">
+        <v>9</v>
+      </c>
+      <c r="N16" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O16" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.1636200206280591</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>612</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.1342925608618203</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.0232259319581084</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.192947480394298</v>
+      </c>
+      <c r="X16" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>156.5</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>151.967978382876</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>154.5</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>156.5</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>151</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>155</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>152.935956765752</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>149.68</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>0.4699349568237442</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>0.5300650431762558</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>-0.0538745669857796</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>0.0062555193667319</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hawai'i Rainbow Warriors vs. Miss Valley St Delta Devils</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Nov 13 12:00AM ET</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Miss Valley St Delta Devils</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>41</v>
+      </c>
+      <c r="F17" t="n">
+        <v>32.85</v>
+      </c>
+      <c r="G17" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.6108053684643127</v>
+      </c>
+      <c r="I17" t="n">
+        <v>41.25</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0813936037584303</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="L17" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="M17" t="n">
+        <v>34</v>
+      </c>
+      <c r="N17" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="O17" t="n">
+        <v>30.6</v>
+      </c>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.0009999999999998001</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.0007367866889574</v>
+      </c>
+      <c r="X17" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>146.5</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>144</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>145.5</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>146.5</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>144</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>144</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>148.374941716665</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>140.98</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>0.4849567874384211</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>0.5150432125615789</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>-0.0388527363711027</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>-0.0064878879168899</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr"/>
+      <c r="AS17" t="inlineStr"/>
+      <c r="AT17" t="inlineStr"/>
+      <c r="AU17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add comprehensive logging and fuzzy matching to game grading
Co-authored-by: trashduty <173416117+trashduty@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/master_game_tracking.xlsx
+++ b/master_game_tracking.xlsx
@@ -2160,7 +2160,11 @@
       <c r="AR16" t="inlineStr"/>
       <c r="AS16" t="inlineStr"/>
       <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2293,7 +2297,11 @@
       <c r="AR17" t="inlineStr"/>
       <c r="AS17" t="inlineStr"/>
       <c r="AT17" t="inlineStr"/>
-      <c r="AU17" t="inlineStr"/>
+      <c r="AU17" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add comprehensive error handling and logging for Excel file creation
Co-authored-by: trashduty <173416117+trashduty@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/master_game_tracking.xlsx
+++ b/master_game_tracking.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU17"/>
+  <dimension ref="A1:AT17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,11 +665,6 @@
           <t>spread_result</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>game_date</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -802,11 +797,6 @@
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr">
-        <is>
-          <t>2025-11-12</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -943,11 +933,6 @@
       <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>2025-11-12</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1084,11 +1069,6 @@
       <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="inlineStr"/>
       <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr">
-        <is>
-          <t>2025-11-12</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1225,11 +1205,6 @@
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>2025-11-12</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1298,11 +1273,6 @@
       <c r="AR6" t="inlineStr"/>
       <c r="AS6" t="inlineStr"/>
       <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1371,11 +1341,6 @@
       <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1444,11 +1409,6 @@
       <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
       <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1517,11 +1477,6 @@
       <c r="AR9" t="inlineStr"/>
       <c r="AS9" t="inlineStr"/>
       <c r="AT9" t="inlineStr"/>
-      <c r="AU9" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -1590,11 +1545,6 @@
       <c r="AR10" t="inlineStr"/>
       <c r="AS10" t="inlineStr"/>
       <c r="AT10" t="inlineStr"/>
-      <c r="AU10" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -1663,11 +1613,6 @@
       <c r="AR11" t="inlineStr"/>
       <c r="AS11" t="inlineStr"/>
       <c r="AT11" t="inlineStr"/>
-      <c r="AU11" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -1736,11 +1681,6 @@
       <c r="AR12" t="inlineStr"/>
       <c r="AS12" t="inlineStr"/>
       <c r="AT12" t="inlineStr"/>
-      <c r="AU12" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -1809,11 +1749,6 @@
       <c r="AR13" t="inlineStr"/>
       <c r="AS13" t="inlineStr"/>
       <c r="AT13" t="inlineStr"/>
-      <c r="AU13" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -1882,11 +1817,6 @@
       <c r="AR14" t="inlineStr"/>
       <c r="AS14" t="inlineStr"/>
       <c r="AT14" t="inlineStr"/>
-      <c r="AU14" t="inlineStr">
-        <is>
-          <t>2025-11-11</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2019,11 +1949,6 @@
       <c r="AR15" t="inlineStr"/>
       <c r="AS15" t="inlineStr"/>
       <c r="AT15" t="inlineStr"/>
-      <c r="AU15" t="inlineStr">
-        <is>
-          <t>2025-11-12</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2160,11 +2085,6 @@
       <c r="AR16" t="inlineStr"/>
       <c r="AS16" t="inlineStr"/>
       <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="inlineStr">
-        <is>
-          <t>2025-11-12</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2297,11 +2217,6 @@
       <c r="AR17" t="inlineStr"/>
       <c r="AS17" t="inlineStr"/>
       <c r="AT17" t="inlineStr"/>
-      <c r="AU17" t="inlineStr">
-        <is>
-          <t>2025-11-13</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3123,7 +3038,11 @@
       <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3260,7 +3179,11 @@
       <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
       <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>